<commit_message>
Saved Changes To Excel File
</commit_message>
<xml_diff>
--- a/FrameworkTest/ExcelData/LoginInfo.xlsx
+++ b/FrameworkTest/ExcelData/LoginInfo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grn_a\eclipse-workspace\FrameworkTest\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grn_a\git\FrameworkTestRepo\FrameworkTest\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7C0E91-1BF0-4D4E-B853-F624D9D78895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8A3D8A-EFDB-451C-AC27-5E71C5579FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,7 +363,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>